<commit_message>
done lots of analysis
</commit_message>
<xml_diff>
--- a/study2/analysis/old/participant_design.xlsx
+++ b/study2/analysis/old/participant_design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27900" yWindow="3180" windowWidth="19200" windowHeight="14280" tabRatio="500" activeTab="2"/>
+    <workbookView minimized="1" xWindow="25600" yWindow="0" windowWidth="19200" windowHeight="21160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="D + O" sheetId="1" r:id="rId1"/>
@@ -240,8 +240,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,7 +286,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -298,6 +302,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -313,6 +319,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3339,8 +3347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3348,6 +3356,7 @@
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12" customWidth="1"/>

</xml_diff>